<commit_message>
Added put request for TestInfo Grid layout API
</commit_message>
<xml_diff>
--- a/BloodstreamAPI/testData/gridLayout.xlsx
+++ b/BloodstreamAPI/testData/gridLayout.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908E6B96-AFFF-43BE-AAF0-840C71CA017B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{514AA16D-B906-49B0-A58F-288DA03AB023}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="715" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="5745" tabRatio="715" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getTestInfoGridLayout" sheetId="2" r:id="rId1"/>
     <sheet name="getDonationInfoGridLayout" sheetId="3" r:id="rId2"/>
     <sheet name="putDonationInfogridLayout" sheetId="7" r:id="rId3"/>
+    <sheet name="putTestInfogridLayout" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:O17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="14">
   <si>
     <t>GroupStatus</t>
   </si>
@@ -436,17 +438,17 @@
       <selection sqref="A1:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.26953125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="26.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
@@ -455,7 +457,7 @@
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
@@ -472,7 +474,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -483,14 +485,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
@@ -499,7 +501,7 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -516,7 +518,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
@@ -527,14 +529,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
@@ -543,7 +545,7 @@
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
@@ -560,7 +562,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -571,7 +573,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
     </row>
   </sheetData>
@@ -593,15 +595,15 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.453125" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
     <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
@@ -610,7 +612,7 @@
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
@@ -627,7 +629,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
@@ -638,14 +640,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
@@ -654,7 +656,7 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -671,7 +673,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -682,14 +684,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
@@ -698,7 +700,7 @@
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
@@ -715,7 +717,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
@@ -740,17 +742,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2FC9B42-5356-4D66-ABF8-4EF2DFAF1ABA}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection sqref="A1:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="45.90625" customWidth="1"/>
-    <col min="5" max="5" width="22.7265625" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
@@ -759,7 +761,7 @@
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
@@ -776,7 +778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
@@ -787,14 +789,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
@@ -803,7 +805,7 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -820,7 +822,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -831,14 +833,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
@@ -847,7 +849,7 @@
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -864,7 +866,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
@@ -875,8 +877,156 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A9:E9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928751EB-AEE1-424B-BB73-34EDBDBF6E22}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="31" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:E1"/>

</xml_diff>